<commit_message>
update the scores in weeport_final2
</commit_message>
<xml_diff>
--- a/score1.xlsx
+++ b/score1.xlsx
@@ -466,8 +466,8 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1272,6 +1272,30 @@
       <c r="C27">
         <v>2</v>
       </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>9</v>
+      </c>
+      <c r="I27">
+        <v>13</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>